<commit_message>
Quick fix on link
</commit_message>
<xml_diff>
--- a/gdp/twogoodtwoperiod.xlsx
+++ b/gdp/twogoodtwoperiod.xlsx
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dietz/Dropbox/Project/StudyGuide/gdp/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5678A6E-1FA9-1145-8B18-E00AA84CE412}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19380" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Raw data</t>
   </si>
@@ -44,22 +61,29 @@
   </si>
   <si>
     <t>Ratio Y2019/Y2018 using Fisher Formula</t>
+  </si>
+  <si>
+    <t>2019(s)</t>
+  </si>
+  <si>
+    <t>2018(t)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -69,43 +93,48 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -295,28 +324,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.57"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -333,84 +367,84 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>2018.0</v>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B4" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F5" si="1">B4*C4+D4*E4</f>
+        <f t="shared" ref="F4:F5" si="0">B4*C4+D4*E4</f>
         <v>30</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>2019.0</v>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>8.0</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>4.0</v>
+        <v>50</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="B8" s="3">
-        <f t="shared" ref="B8:E8" si="2">B4</f>
+        <f t="shared" ref="B8:E8" si="1">B4</f>
         <v>2</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" ref="F8:F9" si="3">B8*C8+D8*E8</f>
+        <f t="shared" ref="F8:F9" si="2">B8*C8+D8*E8</f>
         <v>30</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="B9" s="3">
         <f>B4</f>
@@ -418,7 +452,7 @@
       </c>
       <c r="C9" s="4">
         <f>C5</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3">
         <f>D4</f>
@@ -426,25 +460,25 @@
       </c>
       <c r="E9" s="4">
         <f>E5</f>
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="3"/>
-        <v>36</v>
+        <f t="shared" si="2"/>
+        <v>290</v>
       </c>
       <c r="H9" s="5">
         <f>F9/F8</f>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>9.6666666666666661</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="B12" s="3">
         <f>B5</f>
@@ -463,16 +497,16 @@
         <v>2</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" ref="F12:F13" si="5">B12*C12+D12*E12</f>
+        <f t="shared" ref="F12:F13" si="3">B12*C12+D12*E12</f>
         <v>44</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:E13" si="4">B5</f>
@@ -480,7 +514,7 @@
       </c>
       <c r="C13" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="4"/>
@@ -488,29 +522,29 @@
       </c>
       <c r="E13" s="4">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="5"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>180</v>
       </c>
       <c r="H13" s="6">
         <f>F13/F12</f>
-        <v>0.9090909091</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>4.0909090909090908</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H17" s="6">
         <f>SQRT(H9*H13)</f>
-        <v>1.044465936</v>
+        <v>6.2885176747350036</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>